<commit_message>
v03 - added restrictions table and notes
</commit_message>
<xml_diff>
--- a/restrictions.xlsx
+++ b/restrictions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\MASTER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6C4734-897C-4389-B359-584B14FEF047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332393EA-D4A1-4329-B175-5B95240F0E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="555" yWindow="2040" windowWidth="24225" windowHeight="8310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1095" yWindow="3435" windowWidth="24225" windowHeight="8310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -273,7 +273,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="O4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="O4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6242,12 +6242,12 @@
   <dimension ref="A1:AI10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="L1" sqref="L1:V1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="12" max="22" width="9.140625" customWidth="1"/>
+    <col min="12" max="22" width="9.140625" hidden="1" customWidth="1"/>
     <col min="35" max="35" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6423,8 +6423,8 @@
         <v>0</v>
       </c>
       <c r="AI2" s="4" t="str">
-        <f>AF2&amp;AE2&amp;AD2&amp;AC2&amp;AB2&amp;AA2&amp;Z2&amp;Y2&amp;X2</f>
-        <v>001001111</v>
+        <f>"0b"&amp;AF2&amp;AE2&amp;AD2&amp;AC2&amp;AB2&amp;AA2&amp;Z2&amp;Y2&amp;X2</f>
+        <v>0b001001111</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
@@ -6506,8 +6506,8 @@
         <v>1</v>
       </c>
       <c r="AI3" s="6" t="str">
-        <f t="shared" ref="AI3:AI10" si="3">AF3&amp;AE3&amp;AD3&amp;AC3&amp;AB3&amp;AA3&amp;Z3&amp;Y3&amp;X3</f>
-        <v>001000011</v>
+        <f t="shared" ref="AI3:AI10" si="3">"0b"&amp;AF3&amp;AE3&amp;AD3&amp;AC3&amp;AB3&amp;AA3&amp;Z3&amp;Y3&amp;X3</f>
+        <v>0b001000011</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
@@ -6526,7 +6526,7 @@
         <v>0</v>
       </c>
       <c r="O4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4" t="b">
         <v>0</v>
@@ -6559,7 +6559,7 @@
       </c>
       <c r="Z4">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA4">
         <f t="shared" si="2"/>
@@ -6590,7 +6590,7 @@
       </c>
       <c r="AI4" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>000000101</v>
+        <v>0b000000001</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
@@ -6673,7 +6673,7 @@
       </c>
       <c r="AI5" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>000011001</v>
+        <v>0b000011001</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
@@ -6756,7 +6756,7 @@
       </c>
       <c r="AI6" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>000111000</v>
+        <v>0b000111000</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
@@ -6839,7 +6839,7 @@
       </c>
       <c r="AI7" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>000110000</v>
+        <v>0b000110000</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
@@ -6922,7 +6922,7 @@
       </c>
       <c r="AI8" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>011000011</v>
+        <v>0b011000011</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
@@ -7005,7 +7005,7 @@
       </c>
       <c r="AI9" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>111000000</v>
+        <v>0b111000000</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7095,7 +7095,7 @@
       </c>
       <c r="AI10" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>010000000</v>
+        <v>0b010000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>